<commit_message>
Fixed stevia simper; added genus-level; updated BH adjustment
</commit_message>
<xml_diff>
--- a/Simper_OTU/stevia.hf_krusk_simper.xlsx
+++ b/Simper_OTU/stevia.hf_krusk_simper.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\Simper_OTU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6F5A8A0-29B6-4151-97D6-1FC79D379ABE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B7F7CA68-E5BD-4761-9355-7075E4CC7525}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
@@ -981,10 +981,13 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="89.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>